<commit_message>
Syncing with version 27.0.30744.0
</commit_message>
<xml_diff>
--- a/Apps/W1/SubscriptionBilling/App/Customer Contracts/Reports/OverviewOfContractComponents.xlsx
+++ b/Apps/W1/SubscriptionBilling/App/Customer Contracts/Reports/OverviewOfContractComponents.xlsx
@@ -1,51 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <x:workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\BCSubscriptionBilling\src\SubscriptionBilling\App\Customer Contracts\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14792718-4D88-4CCE-871E-E0E1EC736E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="$ContractComponents$" sheetId="6" r:id="rId1"/>
-    <sheet name="TranslationData" sheetId="2" r:id="rId2"/>
-    <sheet name="CaptionData" sheetId="3" r:id="rId3"/>
-    <sheet name="Aggregated Metadata" sheetId="4" r:id="rId4"/>
-    <sheet name="CustomerContract" sheetId="5" r:id="rId5"/>
-  </sheets>
-  <definedNames>
-    <definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId6"/>
-  </pivotCaches>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+  <x:bookViews>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="$ContractComponents$" sheetId="6" r:id="rId1"/>
+    <x:sheet name="TranslationData" sheetId="2" r:id="rId2"/>
+    <x:sheet name="CaptionData" sheetId="3" r:id="rId3"/>
+    <x:sheet name="Aggregated Metadata" sheetId="4" r:id="rId4"/>
+    <x:sheet name="CustomerContract" sheetId="5" r:id="rId5"/>
+  </x:sheets>
+  <x:definedNames>
+    <x:definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+  </x:definedNames>
+  <x:calcPr calcId="191029"/>
+  <x:pivotCaches>
+    <x:pivotCache cacheId="21" r:id="rId6"/>
+  </x:pivotCaches>
+  <x:extLst>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -55,9 +55,9 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2388,30 +2388,30 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="CustomerContract" displayName="CustomerContract" ref="A1:R2" totalsRowShown="0" headerRowDxfId="74">
-  <autoFilter ref="A1:R2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceObjectNo"/>
-    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceObjectDescription"/>
-    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="UniqueAttribute"/>
-    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceCommitmentDescription"/>
-    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceStartDate"/>
-    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceEndDate"/>
-    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="NextBillingDate"/>
-    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerReference"/>
-    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SerialNo"/>
-    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Quantity"/>
-    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Price"/>
-    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DiscountPct"/>
-    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceAmount"/>
-    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SellToCustomerNo"/>
-    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SellToCustomerName"/>
-    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ContractNo"/>
-    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ContractDescription"/>
-    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ContractType"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="CustomerContract" displayName="CustomerContract" ref="A1:R2" totalsRowShown="0" headerRowDxfId="74" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+  <x:autoFilter ref="A1:R2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <x:tableColumns count="18">
+    <x:tableColumn id="1" name="ServiceObjectNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="2" name="ServiceObjectDescription" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="3" name="UniqueAttribute" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="4" name="ServiceCommitmentDescription" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="5" name="ServiceStartDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="6" name="ServiceEndDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="7" name="NextBillingDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="8" name="CustomerReference" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="9" name="SerialNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="10" name="Quantity" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="11" name="Price" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="12" name="DiscountPct" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="13" name="ServiceAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="14" name="SellToCustomerNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="15" name="SellToCustomerName" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="16" name="ContractNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="17" name="ContractDescription" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="18" name="ContractType" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Syncing with version 27.0.30744.0 (#28292)
Fixes
[AB#560539](https://dynamicssmb2.visualstudio.com/1fcb79e7-ab07-432a-a3c6-6cf5a88ba4a5/_workitems/edit/560539)
</commit_message>
<xml_diff>
--- a/Apps/W1/SubscriptionBilling/App/Customer Contracts/Reports/OverviewOfContractComponents.xlsx
+++ b/Apps/W1/SubscriptionBilling/App/Customer Contracts/Reports/OverviewOfContractComponents.xlsx
@@ -1,51 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <x:workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\BCSubscriptionBilling\src\SubscriptionBilling\App\Customer Contracts\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14792718-4D88-4CCE-871E-E0E1EC736E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="$ContractComponents$" sheetId="6" r:id="rId1"/>
-    <sheet name="TranslationData" sheetId="2" r:id="rId2"/>
-    <sheet name="CaptionData" sheetId="3" r:id="rId3"/>
-    <sheet name="Aggregated Metadata" sheetId="4" r:id="rId4"/>
-    <sheet name="CustomerContract" sheetId="5" r:id="rId5"/>
-  </sheets>
-  <definedNames>
-    <definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-    <definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId6"/>
-  </pivotCaches>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+  <x:bookViews>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="$ContractComponents$" sheetId="6" r:id="rId1"/>
+    <x:sheet name="TranslationData" sheetId="2" r:id="rId2"/>
+    <x:sheet name="CaptionData" sheetId="3" r:id="rId3"/>
+    <x:sheet name="Aggregated Metadata" sheetId="4" r:id="rId4"/>
+    <x:sheet name="CustomerContract" sheetId="5" r:id="rId5"/>
+  </x:sheets>
+  <x:definedNames>
+    <x:definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+    <x:definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none",)</x:definedName>
+  </x:definedNames>
+  <x:calcPr calcId="191029"/>
+  <x:pivotCaches>
+    <x:pivotCache cacheId="21" r:id="rId6"/>
+  </x:pivotCaches>
+  <x:extLst>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -55,9 +55,9 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2388,30 +2388,30 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="CustomerContract" displayName="CustomerContract" ref="A1:R2" totalsRowShown="0" headerRowDxfId="74">
-  <autoFilter ref="A1:R2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceObjectNo"/>
-    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceObjectDescription"/>
-    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="UniqueAttribute"/>
-    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceCommitmentDescription"/>
-    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceStartDate"/>
-    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceEndDate"/>
-    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="NextBillingDate"/>
-    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerReference"/>
-    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SerialNo"/>
-    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Quantity"/>
-    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Price"/>
-    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DiscountPct"/>
-    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ServiceAmount"/>
-    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SellToCustomerNo"/>
-    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SellToCustomerName"/>
-    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ContractNo"/>
-    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ContractDescription"/>
-    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ContractType"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="CustomerContract" displayName="CustomerContract" ref="A1:R2" totalsRowShown="0" headerRowDxfId="74" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+  <x:autoFilter ref="A1:R2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <x:tableColumns count="18">
+    <x:tableColumn id="1" name="ServiceObjectNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="2" name="ServiceObjectDescription" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="3" name="UniqueAttribute" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="4" name="ServiceCommitmentDescription" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="5" name="ServiceStartDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="6" name="ServiceEndDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="7" name="NextBillingDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="8" name="CustomerReference" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="9" name="SerialNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="10" name="Quantity" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="11" name="Price" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="12" name="DiscountPct" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="13" name="ServiceAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="14" name="SellToCustomerNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="15" name="SellToCustomerName" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="16" name="ContractNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="17" name="ContractDescription" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="18" name="ContractType" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>